<commit_message>
Vzpostavil povezavo z Git
</commit_message>
<xml_diff>
--- a/podatki/SvetovnaPrvenstva.xlsx
+++ b/podatki/SvetovnaPrvenstva.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="123820"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Spin\MurA16$\_System\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
@@ -2354,7 +2349,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2415,7 +2410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2518,11 +2513,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBEBEBE"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFBEBEBE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBEBEBE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2563,8 +2571,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2572,13 +2584,21 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2594,9 +2614,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pisarna">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2634,9 +2654,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pisarna">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2671,7 +2691,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2706,7 +2726,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pisarna">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2880,7 +2900,7 @@
   <dimension ref="A1:AM81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T84" sqref="T84"/>
+      <selection activeCell="AI81" sqref="AI81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,7 +2909,8 @@
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" customWidth="1"/>
-    <col min="5" max="7" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="3.42578125" customWidth="1"/>
     <col min="8" max="10" width="4.42578125" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" customWidth="1"/>
     <col min="12" max="13" width="4.5703125" customWidth="1"/>
@@ -8088,34 +8109,34 @@
       <c r="C75" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D75" s="16">
-        <v>3</v>
-      </c>
-      <c r="E75" s="16"/>
-      <c r="F75" s="5">
+      <c r="D75" s="21">
+        <v>3</v>
+      </c>
+      <c r="E75" s="18">
         <v>0</v>
       </c>
-      <c r="G75" s="5">
+      <c r="F75" s="18">
         <v>0</v>
       </c>
-      <c r="H75" s="5">
-        <v>3</v>
-      </c>
-      <c r="I75" s="5">
+      <c r="G75" s="18">
+        <v>3</v>
+      </c>
+      <c r="H75" s="18">
         <v>0</v>
       </c>
-      <c r="J75" s="5">
+      <c r="I75" s="18">
         <v>9</v>
+      </c>
+      <c r="J75" s="18">
+        <v>0</v>
       </c>
       <c r="K75" s="5">
         <v>0</v>
       </c>
-      <c r="L75" s="5">
-        <v>0</v>
-      </c>
-      <c r="M75" s="5">
-        <v>1</v>
-      </c>
+      <c r="L75" s="14">
+        <v>1</v>
+      </c>
+      <c r="M75" s="5"/>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
@@ -8137,8 +8158,8 @@
       </c>
       <c r="AE75" s="4"/>
       <c r="AF75" s="4"/>
-      <c r="AG75" s="4"/>
-      <c r="AH75" s="17"/>
+      <c r="AG75" s="17"/>
+      <c r="AH75" s="15"/>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -8150,34 +8171,34 @@
       <c r="C76" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D76" s="18">
-        <v>3</v>
-      </c>
-      <c r="E76" s="18"/>
-      <c r="F76" s="2">
+      <c r="D76" s="22">
+        <v>3</v>
+      </c>
+      <c r="E76" s="19">
         <v>0</v>
       </c>
-      <c r="G76" s="2">
+      <c r="F76" s="19">
         <v>0</v>
       </c>
-      <c r="H76" s="2">
-        <v>3</v>
-      </c>
-      <c r="I76" s="2">
+      <c r="G76" s="19">
+        <v>3</v>
+      </c>
+      <c r="H76" s="19">
         <v>2</v>
       </c>
-      <c r="J76" s="1">
+      <c r="I76" s="1">
         <v>14</v>
+      </c>
+      <c r="J76" s="19">
+        <v>0</v>
       </c>
       <c r="K76" s="2">
         <v>0</v>
       </c>
-      <c r="L76" s="2">
-        <v>0</v>
-      </c>
-      <c r="M76" s="2">
-        <v>1</v>
-      </c>
+      <c r="L76" s="16">
+        <v>1</v>
+      </c>
+      <c r="M76" s="2"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
       <c r="P76" s="6"/>
@@ -8199,8 +8220,8 @@
       <c r="AD76" s="6"/>
       <c r="AE76" s="6"/>
       <c r="AF76" s="6"/>
-      <c r="AG76" s="6"/>
-      <c r="AH76" s="17"/>
+      <c r="AG76" s="17"/>
+      <c r="AH76" s="15"/>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
@@ -8212,34 +8233,34 @@
       <c r="C77" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D77" s="16">
-        <v>3</v>
-      </c>
-      <c r="E77" s="16"/>
-      <c r="F77" s="5">
+      <c r="D77" s="21">
+        <v>3</v>
+      </c>
+      <c r="E77" s="18">
         <v>0</v>
       </c>
-      <c r="G77" s="5">
+      <c r="F77" s="18">
         <v>0</v>
       </c>
-      <c r="H77" s="5">
-        <v>3</v>
-      </c>
-      <c r="I77" s="5">
+      <c r="G77" s="18">
+        <v>3</v>
+      </c>
+      <c r="H77" s="18">
         <v>0</v>
       </c>
-      <c r="J77" s="3">
+      <c r="I77" s="3">
         <v>14</v>
+      </c>
+      <c r="J77" s="18">
+        <v>0</v>
       </c>
       <c r="K77" s="5">
         <v>0</v>
       </c>
-      <c r="L77" s="5">
-        <v>0</v>
-      </c>
-      <c r="M77" s="5">
-        <v>1</v>
-      </c>
+      <c r="L77" s="14">
+        <v>1</v>
+      </c>
+      <c r="M77" s="5"/>
       <c r="N77" s="4"/>
       <c r="O77" s="4"/>
       <c r="P77" s="4"/>
@@ -8261,8 +8282,8 @@
       <c r="AD77" s="4"/>
       <c r="AE77" s="4"/>
       <c r="AF77" s="4"/>
-      <c r="AG77" s="4"/>
-      <c r="AH77" s="17"/>
+      <c r="AG77" s="17"/>
+      <c r="AH77" s="15"/>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -8274,34 +8295,34 @@
       <c r="C78" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D78" s="18">
+      <c r="D78" s="22">
         <v>6</v>
       </c>
-      <c r="E78" s="18"/>
-      <c r="F78" s="2">
+      <c r="E78" s="19">
         <v>0</v>
       </c>
-      <c r="G78" s="2">
+      <c r="F78" s="19">
         <v>0</v>
       </c>
-      <c r="H78" s="2">
+      <c r="G78" s="19">
         <v>6</v>
       </c>
-      <c r="I78" s="2">
-        <v>1</v>
-      </c>
-      <c r="J78" s="1">
+      <c r="H78" s="19">
+        <v>1</v>
+      </c>
+      <c r="I78" s="1">
         <v>22</v>
+      </c>
+      <c r="J78" s="19">
+        <v>0</v>
       </c>
       <c r="K78" s="2">
         <v>0</v>
       </c>
-      <c r="L78" s="2">
-        <v>0</v>
-      </c>
-      <c r="M78" s="2">
+      <c r="L78" s="16">
         <v>2</v>
       </c>
+      <c r="M78" s="2"/>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
       <c r="P78" s="6"/>
@@ -8325,141 +8346,130 @@
       <c r="AD78" s="6"/>
       <c r="AE78" s="6"/>
       <c r="AF78" s="6"/>
-      <c r="AG78" s="6"/>
-      <c r="AH78" s="17"/>
+      <c r="AH78" s="15"/>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="15">
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="17">
         <v>836</v>
       </c>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="15"/>
-      <c r="O79" s="15"/>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="15"/>
-      <c r="R79" s="15"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="15"/>
-      <c r="U79" s="15"/>
-      <c r="V79" s="15"/>
-      <c r="W79" s="15"/>
-      <c r="X79" s="15"/>
-      <c r="Y79" s="15"/>
-      <c r="Z79" s="15"/>
-      <c r="AA79" s="15"/>
-      <c r="AB79" s="15"/>
-      <c r="AC79" s="15"/>
-      <c r="AD79" s="15"/>
-      <c r="AE79" s="15"/>
-      <c r="AF79" s="15"/>
-      <c r="AG79" s="15"/>
-      <c r="AH79" s="15"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="17"/>
+      <c r="R79" s="17"/>
+      <c r="S79" s="17"/>
+      <c r="T79" s="17"/>
+      <c r="U79" s="17"/>
+      <c r="V79" s="17"/>
+      <c r="W79" s="17"/>
+      <c r="X79" s="17"/>
+      <c r="Y79" s="17"/>
+      <c r="Z79" s="17"/>
+      <c r="AA79" s="17"/>
+      <c r="AB79" s="17"/>
+      <c r="AC79" s="17"/>
+      <c r="AD79" s="17"/>
+      <c r="AE79" s="17"/>
+      <c r="AF79" s="17"/>
+      <c r="AH79" s="17"/>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="15">
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="17">
         <v>2379</v>
       </c>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="15"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="15"/>
-      <c r="U80" s="15"/>
-      <c r="V80" s="15"/>
-      <c r="W80" s="15"/>
-      <c r="X80" s="15"/>
-      <c r="Y80" s="15"/>
-      <c r="Z80" s="15"/>
-      <c r="AA80" s="15"/>
-      <c r="AB80" s="15"/>
-      <c r="AC80" s="15"/>
-      <c r="AD80" s="15"/>
-      <c r="AE80" s="15"/>
-      <c r="AF80" s="15"/>
-      <c r="AG80" s="15"/>
-      <c r="AH80" s="15"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="17"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="17"/>
+      <c r="R80" s="17"/>
+      <c r="S80" s="17"/>
+      <c r="T80" s="17"/>
+      <c r="U80" s="17"/>
+      <c r="V80" s="17"/>
+      <c r="W80" s="17"/>
+      <c r="X80" s="17"/>
+      <c r="Y80" s="17"/>
+      <c r="Z80" s="17"/>
+      <c r="AA80" s="17"/>
+      <c r="AB80" s="17"/>
+      <c r="AC80" s="17"/>
+      <c r="AD80" s="17"/>
+      <c r="AE80" s="17"/>
+      <c r="AF80" s="17"/>
+      <c r="AH80" s="17"/>
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
+      <c r="A81" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="15">
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="17">
         <v>2.85</v>
       </c>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="15"/>
-      <c r="V81" s="15"/>
-      <c r="W81" s="15"/>
-      <c r="X81" s="15"/>
-      <c r="Y81" s="15"/>
-      <c r="Z81" s="15"/>
-      <c r="AA81" s="15"/>
-      <c r="AB81" s="15"/>
-      <c r="AC81" s="15"/>
-      <c r="AD81" s="15"/>
-      <c r="AE81" s="15"/>
-      <c r="AF81" s="15"/>
-      <c r="AG81" s="15"/>
-      <c r="AH81" s="15"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+      <c r="J81" s="17"/>
+      <c r="K81" s="17"/>
+      <c r="L81" s="17"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
+      <c r="Q81" s="17"/>
+      <c r="R81" s="17"/>
+      <c r="S81" s="17"/>
+      <c r="T81" s="17"/>
+      <c r="U81" s="17"/>
+      <c r="V81" s="17"/>
+      <c r="W81" s="17"/>
+      <c r="X81" s="17"/>
+      <c r="Y81" s="17"/>
+      <c r="Z81" s="17"/>
+      <c r="AA81" s="17"/>
+      <c r="AB81" s="17"/>
+      <c r="AC81" s="17"/>
+      <c r="AD81" s="17"/>
+      <c r="AE81" s="17"/>
+      <c r="AF81" s="17"/>
+      <c r="AH81" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="3">
     <mergeCell ref="A80:D80"/>
-    <mergeCell ref="E80:AH80"/>
     <mergeCell ref="A81:D81"/>
-    <mergeCell ref="E81:AH81"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
     <mergeCell ref="A79:D79"/>
-    <mergeCell ref="E79:AH79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>